<commit_message>
Updated Data Persistence in response to TA comments
For the 5th time...
</commit_message>
<xml_diff>
--- a/docs/Data Persistence.xlsx
+++ b/docs/Data Persistence.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="0" windowWidth="28800" windowHeight="16580"/>
+    <workbookView xWindow="1065" yWindow="0" windowWidth="20670" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
   <si>
     <t>UserName</t>
   </si>
@@ -54,12 +54,6 @@
     <t>DueDate</t>
   </si>
   <si>
-    <t>PenaltyMultiplier</t>
-  </si>
-  <si>
-    <t>BonusMultiplier</t>
-  </si>
-  <si>
     <t>SolutionPath</t>
   </si>
   <si>
@@ -84,68 +78,113 @@
     <t>Float</t>
   </si>
   <si>
-    <t>Assigned TA</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Coursename</t>
-  </si>
-  <si>
-    <t>Activityname</t>
-  </si>
-  <si>
     <t>InstructorName</t>
   </si>
   <si>
     <t>Activity table</t>
   </si>
   <si>
-    <t>InstructorId</t>
-  </si>
-  <si>
-    <t>Courseid</t>
-  </si>
-  <si>
-    <t>MarkerName</t>
-  </si>
-  <si>
-    <t>Markerid</t>
-  </si>
-  <si>
-    <t>instructorid</t>
-  </si>
-  <si>
     <t>StartDate</t>
   </si>
   <si>
-    <t>Employeeid</t>
-  </si>
-  <si>
     <t>Course Table</t>
   </si>
   <si>
-    <t>Assignment Marking Table</t>
-  </si>
-  <si>
     <t>Username Table</t>
   </si>
   <si>
-    <t>Instructor Table</t>
-  </si>
-  <si>
-    <t>TA Table</t>
+    <t>Activity Marking Table</t>
+  </si>
+  <si>
+    <t>InstructorID</t>
+  </si>
+  <si>
+    <t>MarkerID</t>
+  </si>
+  <si>
+    <t>ActivitName</t>
+  </si>
+  <si>
+    <t>EmployeeID</t>
+  </si>
+  <si>
+    <t>AssignedTA</t>
+  </si>
+  <si>
+    <t>Penalty Bonus Table</t>
+  </si>
+  <si>
+    <t>BonusDate1</t>
+  </si>
+  <si>
+    <t>BonusDate2</t>
+  </si>
+  <si>
+    <t>BonusDate3</t>
+  </si>
+  <si>
+    <t>PenaltyDate1</t>
+  </si>
+  <si>
+    <t>PenaltyDate2</t>
+  </si>
+  <si>
+    <t>PenaltyDate3</t>
+  </si>
+  <si>
+    <t>BonusValue1</t>
+  </si>
+  <si>
+    <t>BonusValue2</t>
+  </si>
+  <si>
+    <t>BonusValue3</t>
+  </si>
+  <si>
+    <t>PenaltyValue1</t>
+  </si>
+  <si>
+    <t>PenaltyValue3</t>
+  </si>
+  <si>
+    <t>PenaltyValue2</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Rubric Table</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>StudentName</t>
+  </si>
+  <si>
+    <t>RubricDesc</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Student To Group Table</t>
+  </si>
+  <si>
+    <t>Student Marks Table</t>
+  </si>
+  <si>
+    <t>RubricEntry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,16 +224,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -281,6 +350,21 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -293,7 +377,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -306,13 +390,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -323,7 +412,80 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="46">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -352,34 +514,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color auto="1"/>
@@ -437,34 +571,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color auto="1"/>
@@ -495,6 +601,21 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
@@ -517,6 +638,40 @@
         <left style="thin">
           <color auto="1"/>
         </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
         <right/>
         <top style="thin">
           <color auto="1"/>
@@ -608,54 +763,6 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
           <color auto="1"/>
@@ -673,6 +780,22 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -683,19 +806,15 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -814,22 +933,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -858,102 +961,18 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -961,34 +980,6 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1127,6 +1118,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -1134,18 +1134,21 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1162,83 +1165,59 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:E3" totalsRowShown="0" headerRowDxfId="43" headerRowBorderDxfId="50" tableBorderDxfId="51" totalsRowBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:E3" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="A2:E3"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="UserName" dataDxfId="48"/>
-    <tableColumn id="2" name="Employeeid" dataDxfId="47"/>
-    <tableColumn id="3" name="Password" dataDxfId="46"/>
-    <tableColumn id="4" name="AccountType" dataDxfId="45"/>
-    <tableColumn id="5" name="BlockAccountFlag" dataDxfId="44"/>
+    <tableColumn id="1" name="UserName" dataDxfId="41"/>
+    <tableColumn id="2" name="EmployeeID" dataDxfId="40"/>
+    <tableColumn id="3" name="Password" dataDxfId="39"/>
+    <tableColumn id="4" name="AccountType" dataDxfId="38"/>
+    <tableColumn id="5" name="BlockAccountFlag" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A7:B8" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="41" tableBorderDxfId="42" totalsRowBorderDxfId="40">
-  <autoFilter ref="A7:B8"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="ActivityName" dataDxfId="39"/>
-    <tableColumn id="2" name="ActivityDesc" dataDxfId="38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A17:I18" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+  <autoFilter ref="A17:I18"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="UserName" dataDxfId="22"/>
+    <tableColumn id="2" name="CourseID" dataDxfId="21"/>
+    <tableColumn id="3" name="ActivitName" dataDxfId="20"/>
+    <tableColumn id="11" name="ActivityDesc" dataDxfId="15"/>
+    <tableColumn id="5" name="DueDate" dataDxfId="19"/>
+    <tableColumn id="6" name="Grade" dataDxfId="14"/>
+    <tableColumn id="8" name="SolutionPath" dataDxfId="18"/>
+    <tableColumn id="9" name="TestInputPath" dataDxfId="17"/>
+    <tableColumn id="10" name="AssignedTA" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A12:H13" totalsRowShown="0" headerRowBorderDxfId="35" tableBorderDxfId="36" totalsRowBorderDxfId="34">
-  <autoFilter ref="A12:H13"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A12:G13" totalsRowShown="0" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="A12:G13"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="CourseID" dataDxfId="33"/>
-    <tableColumn id="2" name="Coursename" dataDxfId="32"/>
-    <tableColumn id="3" name="MarkerName" dataDxfId="31"/>
-    <tableColumn id="4" name="Markerid" dataDxfId="30"/>
-    <tableColumn id="5" name="InstructorName" dataDxfId="29"/>
-    <tableColumn id="6" name="instructorid" dataDxfId="28"/>
-    <tableColumn id="7" name="StartDate" dataDxfId="27"/>
-    <tableColumn id="8" name="EndDate" dataDxfId="26"/>
+    <tableColumn id="2" name="CourseName" dataDxfId="32"/>
+    <tableColumn id="4" name="MarkerID" dataDxfId="31"/>
+    <tableColumn id="5" name="InstructorName" dataDxfId="30"/>
+    <tableColumn id="6" name="InstructorID" dataDxfId="29"/>
+    <tableColumn id="7" name="StartDate" dataDxfId="28"/>
+    <tableColumn id="8" name="EndDate" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A17:J18" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="24" tableBorderDxfId="25" totalsRowBorderDxfId="23">
-  <autoFilter ref="A17:J18"/>
-  <tableColumns count="10">
-    <tableColumn id="1" name="Username" dataDxfId="22"/>
-    <tableColumn id="2" name="Courseid" dataDxfId="21"/>
-    <tableColumn id="3" name="Activityname" dataDxfId="20"/>
-    <tableColumn id="4" name="CourseName" dataDxfId="19"/>
-    <tableColumn id="5" name="DueDate" dataDxfId="18"/>
-    <tableColumn id="6" name="PenaltyMultiplier" dataDxfId="17"/>
-    <tableColumn id="7" name="BonusMultiplier" dataDxfId="16"/>
-    <tableColumn id="8" name="SolutionPath" dataDxfId="15"/>
-    <tableColumn id="9" name="TestInputPath" dataDxfId="14"/>
-    <tableColumn id="10" name="Assigned TA" dataDxfId="13"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A21:B22" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
-  <autoFilter ref="A21:B22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A7:B8" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
+  <autoFilter ref="A7:B8"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="InstructorId" dataDxfId="8"/>
-    <tableColumn id="2" name="InstructorName" dataDxfId="7"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A25:B26" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
-  <autoFilter ref="A25:B26"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Markerid" dataDxfId="2"/>
-    <tableColumn id="2" name="MarkerName" dataDxfId="1"/>
+    <tableColumn id="1" name="ActivityName" dataDxfId="1"/>
+    <tableColumn id="2" name="ActivityDesc" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1499,7 +1478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1507,38 +1486,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="19.5" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
@@ -1550,29 +1529,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="E3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1580,193 +1559,308 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="14" t="s">
-        <v>14</v>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>16</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="K22" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="L22" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="M22" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="L23" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>14</v>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
-  <tableParts count="6">
-    <tablePart r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
-    <tablePart r:id="rId6"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>